<commit_message>
Added my name and stuff
</commit_message>
<xml_diff>
--- a/git test file.xlsx
+++ b/git test file.xlsx
@@ -16,6 +16,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>Sturek</t>
+  </si>
+  <si>
+    <t>doin stuff</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,12 +400,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>